<commit_message>
commited on 15 Feb 2022
</commit_message>
<xml_diff>
--- a/SSFA2021.xlsx
+++ b/SSFA2021.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcollins/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcollins/GitHub/SnapShot_USA_CamTrap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605748A3-22F7-1748-BB6D-30772707226F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D57F7DB-FA4E-8C49-B61A-EA09108FA6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="25040" windowHeight="14420" xr2:uid="{36C54280-45A2-EB4C-8F2D-57B48137AB3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$J$1:$J$1856</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14853" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14853" uniqueCount="88">
   <si>
     <t>deployment_id</t>
   </si>
@@ -298,12 +301,6 @@
   </si>
   <si>
     <t>Human-Pedestrian</t>
-  </si>
-  <si>
-    <t>lupus</t>
-  </si>
-  <si>
-    <t>Grey Wolf</t>
   </si>
 </sst>
 </file>
@@ -659,7 +656,7 @@
   <dimension ref="A1:M1856"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E913" sqref="E913"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33748,10 +33745,10 @@
         <v>50</v>
       </c>
       <c r="I807" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="J807" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="K807" s="1">
         <v>44447.089618055557</v>
@@ -76773,6 +76770,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="J1:J1856" xr:uid="{178DC9D3-2295-9B4C-9F69-182ACD5878F4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>